<commit_message>
20251119 es2pr capping attempt
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202509/Developed Market.xlsx
+++ b/GUI + Reviews/202509/Developed Market.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\PM-Indices-IndexOperations\Review Files\202509\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/202509/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3824C6D6-0B3E-4363-AA41-DED8F75E71B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{3824C6D6-0B3E-4363-AA41-DED8F75E71B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47F08284-D63B-43C8-939C-6729980155DE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{714B9672-26A4-408E-A222-7E8DF6A256AB}"/>
+    <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15720" xr2:uid="{714B9672-26A4-408E-A222-7E8DF6A256AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14645,8 +14645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06955FEC-7ADA-4129-AB4F-542F236A2C83}">
   <dimension ref="A1:K1539"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1373" workbookViewId="0">
-      <selection activeCell="E1394" sqref="E1394"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>